<commit_message>
fixed spacing in excel output
</commit_message>
<xml_diff>
--- a/coded_(3)_(3,9,9,9)_ 1.xlsx
+++ b/coded_(3)_(3,9,9,9)_ 1.xlsx
@@ -393,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:Q4"/>
+  <dimension ref="B1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -449,156 +449,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:17">
-      <c r="B2">
-        <v>503</v>
-      </c>
-      <c r="C2">
-        <v>521</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17">
-      <c r="B3">
-        <v>503</v>
-      </c>
-      <c r="C3">
-        <v>521</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17">
-      <c r="B4">
-        <v>503</v>
-      </c>
-      <c r="C4">
-        <v>521</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed excel output, fixed compiler order
</commit_message>
<xml_diff>
--- a/coded_(3)_(3,9,9,9)_ 1.xlsx
+++ b/coded_(3)_(3,9,9,9)_ 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>0000</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>1011</t>
+  </si>
+  <si>
+    <t>Length: 3</t>
+  </si>
+  <si>
+    <t>Compiler: 0</t>
   </si>
 </sst>
 </file>
@@ -393,13 +399,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:Q4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:17">
+    <row r="1" spans="1:17">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -449,12 +455,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:17">
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
       <c r="B2">
-        <v>521</v>
+        <v>472</v>
       </c>
       <c r="C2">
-        <v>503</v>
+        <v>552</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -499,12 +508,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:17">
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
       <c r="B3">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="C3">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -549,12 +561,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:17">
+    <row r="4" spans="1:17">
       <c r="B4">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C4">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D4">
         <v>0</v>

</xml_diff>